<commit_message>
Added additional variables to example data file (exampledata2.xlsx), and added descriptions for the files in the quarto report file.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FA1AC5-FE6F-421E-BC65-6E379E127CAF}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -133,6 +144,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,9 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -577,15 +590,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>